<commit_message>
All functions working, need work on the UI and need to greatly expand the options of ingredients across all subcategories, particularly in the Dessert section
</commit_message>
<xml_diff>
--- a/ChoppedList.xlsx
+++ b/ChoppedList.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stephen.heath\Desktop\Chopped Generator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stephen.heath\Ruby\friendshipbasket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ACFB239-9C0B-464A-86A6-DBD136FB3A4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73542EB-98A1-4282-AF7E-ED5F30600A56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="10" xr2:uid="{8ADFD618-CB20-4DFA-986E-320356274DEA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="9" xr2:uid="{8ADFD618-CB20-4DFA-986E-320356274DEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Entree" sheetId="7" r:id="rId1"/>
@@ -187,9 +187,6 @@
     <t>Agave Nector</t>
   </si>
   <si>
-    <t>Turbino</t>
-  </si>
-  <si>
     <t>Candy Canes</t>
   </si>
   <si>
@@ -320,6 +317,9 @@
   </si>
   <si>
     <t>Sun dried tomatos</t>
+  </si>
+  <si>
+    <t>Raw Sugar</t>
   </si>
 </sst>
 </file>
@@ -683,62 +683,67 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9702B924-94DB-43B2-8002-F56CE8328920}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>82</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -750,7 +755,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1921C64-BFE8-4B5B-8A38-50D7E418CEC5}">
   <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -763,17 +768,17 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
@@ -793,27 +798,27 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -948,7 +953,7 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -968,7 +973,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -993,62 +998,62 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1073,7 +1078,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -1108,32 +1113,32 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1168,17 +1173,17 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1248,10 +1253,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59B33399-3979-4E4E-BA86-CD7D5F9AD645}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1268,7 +1273,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
@@ -1278,12 +1283,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>